<commit_message>
added reactivity to the tracker
</commit_message>
<xml_diff>
--- a/montco-rps/data/RPS Tracker Data.xlsx
+++ b/montco-rps/data/RPS Tracker Data.xlsx
@@ -1,19 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakna\OneDrive\Desktop\MontCo-ReImagining-Public-Safety\montco-rps\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB10EAF-7920-4964-B9D1-D167AB9096F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Actions" sheetId="1" r:id="rId4"/>
-    <sheet state="hidden" name="Actions As Provided 129" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Focus Areas" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Parties" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Progress Updates" sheetId="5" r:id="rId8"/>
+    <sheet name="Actions" sheetId="1" r:id="rId1"/>
+    <sheet name="Actions As Provided 129" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Focus Areas" sheetId="3" r:id="rId3"/>
+    <sheet name="Parties" sheetId="4" r:id="rId4"/>
+    <sheet name="Progress Updates" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Actions!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Actions!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhWq4vzTofNQMdYN5C9ehJJoHS59A=="/>
     </ext>
@@ -22,23 +41,31 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C21">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
 ID#AAAAMQbRpCk
     (2021-04-30 21:39:08)
 This may change during the period the tracker is live.
 	-Natalie Schultz-Henry</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi7+Xw6e+91EiiQexCBbRcUODI63A=="/>
     </ext>
   </extLst>
@@ -46,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="223">
   <si>
     <t>Action #</t>
   </si>
@@ -67,9 +94,6 @@
   </si>
   <si>
     <t>Anticipated Timeline</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>Montgomery County Police Department (MCPD) Programs</t>
@@ -122,18 +146,18 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>Report</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Roboto"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve"> published evaluating Montgomery County's capacity to respond to mental health situations. Overall, OLO found that the County uses several research-supported practices to respond to mental health situations and is currently working to reduce reliance on law enforcement for crisis response</t>
     </r>
@@ -183,41 +207,41 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF1B2333"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1B2333"/>
-        <sz val="11.0"/>
       </rPr>
       <t>Develop a new Mobile Crisis Team approach, drawing from nationally recognized models like Crisis Assistance Helping Out On The Streets (</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF1B2333"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1B2333"/>
-        <sz val="11.0"/>
       </rPr>
       <t>CAHOOTS</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF1B2333"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1B2333"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve">) and the </t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF1B2333"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1B2333"/>
-        <sz val="11.0"/>
       </rPr>
       <t>Crisis Now</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF1B2333"/>
         <rFont val="Roboto"/>
-        <color rgb="FF1B2333"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve"> programs.</t>
     </r>
@@ -770,118 +794,161 @@
 &lt;/ul&gt;
 &lt;p&gt;&lt;span style="font-size: 16px;"&gt;We have bold plans to reshape Baltimore&amp;rsquo;s government over the coming months. This work will involve unprecedented transparency, accountability, and urgency as we seek to build a Baltimore where every resident can thrive.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
+  <si>
+    <t>Priority Level</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF2A2A2A"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1B2333"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="-webkit-standard"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1B2333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -889,7 +956,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -905,12 +972,19 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -925,6 +999,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -933,6 +1008,7 @@
       <bottom style="thin">
         <color rgb="FFB7B7B7"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -943,169 +1019,147 @@
       <bottom style="thin">
         <color rgb="FFB7B7B7"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1295,32 +1349,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H953"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="15.0" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B17" sqref="B17" pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.86"/>
-    <col customWidth="1" min="2" max="2" width="30.43"/>
-    <col customWidth="1" min="3" max="4" width="53.43"/>
-    <col customWidth="1" min="5" max="5" width="70.29"/>
-    <col customWidth="1" min="6" max="6" width="19.29"/>
-    <col customWidth="1" min="7" max="8" width="19.57"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="4" width="53.42578125" customWidth="1"/>
+    <col min="5" max="5" width="70.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1343,265 +1399,263 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60.75" customHeight="1">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" ht="60.75" customHeight="1">
-      <c r="A2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="93.75" customHeight="1">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3" ht="93.75" customHeight="1">
-      <c r="A3" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="42" customHeight="1">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="89.25" customHeight="1">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45.75" customHeight="1">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="42.0" customHeight="1">
-      <c r="A4" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5" ht="89.25" customHeight="1">
-      <c r="A5" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6" ht="31.5" customHeight="1">
-      <c r="A6" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" ht="45.75" customHeight="1">
-      <c r="A7" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8" ht="31.5" customHeight="1">
-      <c r="A8" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" ht="31.5" customHeight="1">
-      <c r="A9" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10" ht="31.5" customHeight="1">
-      <c r="A10" s="5">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11" ht="31.5" customHeight="1">
-      <c r="A11" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12" ht="31.5" customHeight="1">
-      <c r="A12" s="5">
-        <v>11.0</v>
-      </c>
+      <c r="H11" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1610,10 +1664,10 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2552,767 +2606,772 @@
     <row r="952" ht="15.75" customHeight="1"/>
     <row r="953" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$A$1:$H$12"/>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Please choose from one of the 10 committees." sqref="B2:B12">
-      <formula1>'Focus Areas'!$B$2:$B$7</formula1>
-    </dataValidation>
-  </dataValidations>
+  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5"/>
-    <hyperlink r:id="rId2" ref="D10"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Please choose from one of the 10 committees." xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>'Focus Areas'!$B$2:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="14.43"/>
+    <col min="1" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A7" s="19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" s="19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="C14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="18" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>76</v>
-      </c>
       <c r="B15" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" s="19" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>78</v>
-      </c>
       <c r="B16" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="19" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="19" t="s">
-        <v>92</v>
-      </c>
       <c r="B23" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>97</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="19" t="s">
-        <v>99</v>
-      </c>
       <c r="B26" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>101</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="C28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="C31" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="18" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="19" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="C33" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="18" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A34" s="19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>115</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A38" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="19" t="s">
-        <v>119</v>
-      </c>
       <c r="B38" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A39" s="19" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="C39" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A40" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="C40" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A41" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="19" t="s">
+      <c r="B41" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="19" t="s">
-        <v>126</v>
-      </c>
       <c r="B42" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="20"/>
       <c r="D42" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>127</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>128</v>
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>129</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>130</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
       <c r="A47" s="20"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
       <c r="A48" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="C49" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A50" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="19" t="s">
-        <v>136</v>
-      </c>
       <c r="B50" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" s="20"/>
       <c r="D50" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A52" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="19" t="s">
+      <c r="B52" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A53" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="19" t="s">
+      <c r="B53" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A54" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="19" t="s">
+      <c r="B54" s="18" t="s">
         <v>140</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>141</v>
       </c>
       <c r="C54" s="20"/>
       <c r="D54" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
       <c r="D55" s="20"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B56" s="17"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="18" t="s">
         <v>146</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>147</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -4250,113 +4309,111 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="57.29"/>
-    <col customWidth="1" min="3" max="3" width="61.57"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="4" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="23" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="26" t="s">
+    <row r="3" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="27" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" ht="22.5" customHeight="1">
-      <c r="A4" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="26" t="s">
+    <row r="5" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="24">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="26" t="s">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" ht="22.5" customHeight="1">
-      <c r="A6" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" ht="22.5" customHeight="1">
+    <row r="7" spans="1:3" ht="22.5" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="28"/>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5342,262 +5399,260 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
-    <col customWidth="1" min="2" max="2" width="56.71"/>
-    <col customWidth="1" min="3" max="3" width="45.0"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="29" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="30" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="B2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="31" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A3" s="30" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="B3" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="C3" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="32" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="30" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="B4" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="C4" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="32" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A5" s="30" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="B5" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C5" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="32" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A6" s="30" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="B6" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="32" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A7" s="30" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="B7" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="C7" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="32" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A8" s="30" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="30" t="s">
+      <c r="B8" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C8" s="33" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" s="30" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="A9" s="30" t="s">
+      <c r="B9" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="C9" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="32" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="30" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="30" t="s">
+      <c r="B10" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="32" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A11" s="30" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="30" t="s">
+      <c r="B11" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="C11" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="33" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A12" s="30" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="30" t="s">
+      <c r="B12" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="C12" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="32" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A13" s="30" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="30" t="s">
+      <c r="B13" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="C13" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="C13" s="32" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="30" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="B14" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="C14" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="C14" s="32" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="30" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="30" t="s">
+      <c r="B15" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="C15" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="32" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="30" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="30" t="s">
+      <c r="B16" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="C16" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="C16" s="32" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="30" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="30" t="s">
+      <c r="B17" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="C17" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="32" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A18" s="30" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="30" t="s">
+      <c r="B18" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="C18" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="C18" s="32" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A19" s="30" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="B19" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="C19" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="32" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A20" s="30" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="30" t="s">
+      <c r="B20" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="B20" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -6569,77 +6624,75 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="C5"/>
-    <hyperlink r:id="rId6" ref="C6"/>
-    <hyperlink r:id="rId7" ref="C7"/>
-    <hyperlink r:id="rId8" ref="C8"/>
-    <hyperlink r:id="rId9" ref="C9"/>
-    <hyperlink r:id="rId10" ref="C10"/>
-    <hyperlink r:id="rId11" ref="C11"/>
-    <hyperlink r:id="rId12" ref="C12"/>
-    <hyperlink r:id="rId13" ref="C13"/>
-    <hyperlink r:id="rId14" ref="C14"/>
-    <hyperlink r:id="rId15" ref="C15"/>
-    <hyperlink r:id="rId16" ref="C16"/>
-    <hyperlink r:id="rId17" ref="C17"/>
-    <hyperlink r:id="rId18" ref="C18"/>
-    <hyperlink r:id="rId19" ref="C19"/>
-    <hyperlink r:id="rId20" ref="C20"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId21"/>
-  <legacyDrawing r:id="rId22"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="11.71"/>
-    <col customWidth="1" min="3" max="3" width="77.57"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="77.5703125" customWidth="1"/>
+    <col min="4" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="34" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="35">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36">
+        <v>44251</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="36">
-        <v>44251.0</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="38">
         <f>IF(AND(ISBLANK(B3), ISBLANK(#REF!)),"",$A$2+1)</f>
         <v>2</v>
@@ -6647,499 +6700,499 @@
       <c r="B3" s="39"/>
       <c r="C3" s="40"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="40"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="38"/>
       <c r="B5" s="39"/>
       <c r="C5" s="40"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="38"/>
       <c r="B6" s="39"/>
       <c r="C6" s="40"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="38"/>
       <c r="B7" s="39"/>
       <c r="C7" s="40"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="38"/>
       <c r="B8" s="39"/>
       <c r="C8" s="40"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="38"/>
       <c r="B9" s="39"/>
       <c r="C9" s="40"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="38"/>
       <c r="B10" s="39"/>
       <c r="C10" s="40"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="38"/>
       <c r="B11" s="39"/>
       <c r="C11" s="40"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="38"/>
       <c r="B12" s="39"/>
       <c r="C12" s="40"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="38"/>
       <c r="B13" s="39"/>
       <c r="C13" s="40"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="38"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="38"/>
       <c r="B15" s="41"/>
       <c r="C15" s="42"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="38"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="38"/>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="38"/>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="38"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="38"/>
       <c r="B21" s="39"/>
       <c r="C21" s="40"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="38"/>
       <c r="B22" s="39"/>
       <c r="C22" s="40"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="38"/>
       <c r="B23" s="39"/>
       <c r="C23" s="40"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="38"/>
       <c r="B24" s="39"/>
       <c r="C24" s="40"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="38"/>
       <c r="B25" s="39"/>
       <c r="C25" s="40"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="38"/>
       <c r="B26" s="39"/>
       <c r="C26" s="40"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="38"/>
       <c r="B27" s="39"/>
       <c r="C27" s="40"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="39"/>
       <c r="C28" s="40"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="38"/>
       <c r="B29" s="39"/>
       <c r="C29" s="40"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="38"/>
       <c r="B30" s="39"/>
       <c r="C30" s="40"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="38"/>
       <c r="B31" s="39"/>
       <c r="C31" s="40"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="38"/>
       <c r="B32" s="39"/>
       <c r="C32" s="40"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="A33" s="38"/>
       <c r="B33" s="39"/>
       <c r="C33" s="40"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
       <c r="A34" s="38"/>
       <c r="B34" s="39"/>
       <c r="C34" s="40"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
       <c r="A35" s="38"/>
       <c r="B35" s="39"/>
       <c r="C35" s="40"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
       <c r="A36" s="38"/>
       <c r="B36" s="39"/>
       <c r="C36" s="40"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
       <c r="A37" s="38"/>
       <c r="B37" s="39"/>
       <c r="C37" s="40"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="A38" s="38"/>
       <c r="B38" s="39"/>
       <c r="C38" s="40"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1">
       <c r="A39" s="38"/>
       <c r="B39" s="39"/>
       <c r="C39" s="40"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="A40" s="38"/>
       <c r="B40" s="39"/>
       <c r="C40" s="40"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1">
       <c r="A41" s="38"/>
       <c r="B41" s="39"/>
       <c r="C41" s="40"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1">
       <c r="A42" s="38"/>
       <c r="B42" s="39"/>
       <c r="C42" s="40"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="39"/>
       <c r="C43" s="40"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="A44" s="38"/>
       <c r="B44" s="39"/>
       <c r="C44" s="40"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="39"/>
       <c r="C45" s="40"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="A46" s="38"/>
       <c r="B46" s="39"/>
       <c r="C46" s="40"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="A47" s="38"/>
       <c r="B47" s="39"/>
       <c r="C47" s="40"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="A48" s="38"/>
       <c r="B48" s="39"/>
       <c r="C48" s="40"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="38"/>
       <c r="B49" s="39"/>
       <c r="C49" s="40"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="39"/>
       <c r="C50" s="40"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
       <c r="A51" s="38"/>
       <c r="B51" s="39"/>
       <c r="C51" s="40"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
       <c r="A52" s="38"/>
       <c r="B52" s="39"/>
       <c r="C52" s="40"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
       <c r="A53" s="38"/>
       <c r="B53" s="39"/>
       <c r="C53" s="40"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
       <c r="A54" s="38"/>
       <c r="B54" s="39"/>
       <c r="C54" s="40"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
       <c r="A55" s="38"/>
       <c r="B55" s="39"/>
       <c r="C55" s="40"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="A56" s="38"/>
       <c r="B56" s="39"/>
       <c r="C56" s="40"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="39"/>
       <c r="C57" s="40"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
       <c r="A58" s="38"/>
       <c r="B58" s="39"/>
       <c r="C58" s="40"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
       <c r="A59" s="38"/>
       <c r="B59" s="39"/>
       <c r="C59" s="40"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
       <c r="A60" s="38"/>
       <c r="B60" s="39"/>
       <c r="C60" s="40"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:3" ht="15.75" customHeight="1">
       <c r="A61" s="38"/>
       <c r="B61" s="39"/>
       <c r="C61" s="40"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="39"/>
       <c r="C62" s="40"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:3" ht="15.75" customHeight="1">
       <c r="A63" s="38"/>
       <c r="B63" s="39"/>
       <c r="C63" s="40"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:3" ht="15.75" customHeight="1">
       <c r="A64" s="38"/>
       <c r="B64" s="39"/>
       <c r="C64" s="40"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1">
       <c r="A65" s="38"/>
       <c r="B65" s="39"/>
       <c r="C65" s="40"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1">
       <c r="A66" s="38"/>
       <c r="B66" s="39"/>
       <c r="C66" s="40"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1">
       <c r="A67" s="38"/>
       <c r="B67" s="39"/>
       <c r="C67" s="40"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="39"/>
       <c r="C68" s="40"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
       <c r="A69" s="38"/>
       <c r="B69" s="39"/>
       <c r="C69" s="40"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1">
       <c r="A70" s="38"/>
       <c r="B70" s="39"/>
       <c r="C70" s="40"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1">
       <c r="A71" s="38"/>
       <c r="B71" s="39"/>
       <c r="C71" s="40"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
       <c r="A72" s="38"/>
       <c r="B72" s="39"/>
       <c r="C72" s="40"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="39"/>
       <c r="C73" s="40"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1">
       <c r="A74" s="38"/>
       <c r="B74" s="39"/>
       <c r="C74" s="40"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1">
       <c r="A75" s="38"/>
       <c r="B75" s="39"/>
       <c r="C75" s="40"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1">
       <c r="A76" s="38"/>
       <c r="B76" s="39"/>
       <c r="C76" s="40"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1">
       <c r="A77" s="38"/>
       <c r="B77" s="39"/>
       <c r="C77" s="40"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="39"/>
       <c r="C78" s="40"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1">
       <c r="A79" s="38"/>
       <c r="B79" s="39"/>
       <c r="C79" s="40"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1">
       <c r="A80" s="38"/>
       <c r="B80" s="39"/>
       <c r="C80" s="40"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1">
       <c r="A81" s="38"/>
       <c r="B81" s="39"/>
       <c r="C81" s="40"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1">
       <c r="A82" s="38"/>
       <c r="B82" s="39"/>
       <c r="C82" s="40"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1">
       <c r="A83" s="38"/>
       <c r="B83" s="39"/>
       <c r="C83" s="40"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1">
       <c r="A84" s="38"/>
       <c r="B84" s="39"/>
       <c r="C84" s="40"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1">
       <c r="A85" s="38"/>
       <c r="B85" s="39"/>
       <c r="C85" s="40"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1">
       <c r="A86" s="38"/>
       <c r="B86" s="39"/>
       <c r="C86" s="40"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1">
       <c r="A87" s="38"/>
       <c r="B87" s="39"/>
       <c r="C87" s="40"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1">
       <c r="A88" s="38"/>
       <c r="B88" s="39"/>
       <c r="C88" s="40"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1">
       <c r="A89" s="38"/>
       <c r="B89" s="39"/>
       <c r="C89" s="40"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1">
       <c r="A90" s="38"/>
       <c r="B90" s="39"/>
       <c r="C90" s="40"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1">
       <c r="A91" s="38"/>
       <c r="B91" s="39"/>
       <c r="C91" s="40"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1">
       <c r="A92" s="38"/>
       <c r="B92" s="39"/>
       <c r="C92" s="40"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1">
       <c r="A93" s="38"/>
       <c r="B93" s="39"/>
       <c r="C93" s="40"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1">
       <c r="A94" s="38"/>
       <c r="B94" s="39"/>
       <c r="C94" s="40"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1">
       <c r="A95" s="38"/>
       <c r="B95" s="39"/>
       <c r="C95" s="40"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1">
       <c r="A96" s="38"/>
       <c r="B96" s="39"/>
       <c r="C96" s="40"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1">
       <c r="A97" s="38"/>
       <c r="B97" s="39"/>
       <c r="C97" s="40"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1">
       <c r="A98" s="38"/>
       <c r="B98" s="39"/>
       <c r="C98" s="40"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="39"/>
       <c r="C99" s="40"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="102" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="103" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="104" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="105" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="106" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="107" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="108" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="109" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="110" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="111" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="112" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
     <row r="115" ht="15.75" customHeight="1"/>
@@ -8029,14 +8082,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 12/8/2020" sqref="B2:B99">
-      <formula1>44173.0</formula1>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 12/8/2020" sqref="B2:B99" xr:uid="{00000000-0002-0000-0400-000000000000}">
+      <formula1>44173</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>